<commit_message>
Fix line breaks in surveys
</commit_message>
<xml_diff>
--- a/app/designerFiles/app/config/tables/person/forms/person/person.xlsx
+++ b/app/designerFiles/app/config/tables/person/forms/person/person.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="21840" windowWidth="38640" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -42,6 +42,12 @@
     <font>
       <name val="Arial"/>
       <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
@@ -88,12 +94,12 @@
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -406,35 +412,35 @@
   <dimension ref="A1:AF107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="71" zoomScaleNormal="71">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="6.6640625"/>
-    <col customWidth="1" max="2" min="2" style="2" width="8.6640625"/>
-    <col customWidth="1" max="3" min="3" style="2" width="10.44140625"/>
-    <col customWidth="1" max="4" min="4" style="2" width="8.6640625"/>
-    <col customWidth="1" max="5" min="5" style="2" width="26.44140625"/>
-    <col customWidth="1" max="6" min="6" style="2" width="19.5546875"/>
-    <col customWidth="1" max="7" min="7" style="2" width="21.6640625"/>
-    <col customWidth="1" max="8" min="8" style="2" width="79.33203125"/>
-    <col customWidth="1" max="9" min="9" style="2" width="57.109375"/>
+    <col customWidth="1" max="1" min="1" style="2" width="6.7109375"/>
+    <col customWidth="1" max="2" min="2" style="2" width="8.7109375"/>
+    <col customWidth="1" max="3" min="3" style="2" width="10.42578125"/>
+    <col customWidth="1" max="4" min="4" style="2" width="8.7109375"/>
+    <col customWidth="1" max="5" min="5" style="2" width="26.42578125"/>
+    <col customWidth="1" max="6" min="6" style="2" width="19.5703125"/>
+    <col customWidth="1" max="7" min="7" style="2" width="21.7109375"/>
+    <col customWidth="1" max="8" min="8" style="2" width="79.28515625"/>
+    <col customWidth="1" max="9" min="9" style="2" width="57.140625"/>
     <col customWidth="1" max="10" min="10" style="2" width="13"/>
-    <col customWidth="1" max="11" min="11" style="2" width="20.6640625"/>
-    <col customWidth="1" max="12" min="12" style="2" width="14.109375"/>
-    <col customWidth="1" max="13" min="13" style="2" width="17.88671875"/>
-    <col customWidth="1" max="14" min="14" style="2" width="18.33203125"/>
+    <col customWidth="1" max="11" min="11" style="2" width="20.7109375"/>
+    <col customWidth="1" max="12" min="12" style="2" width="14.140625"/>
+    <col customWidth="1" max="13" min="13" style="2" width="17.85546875"/>
+    <col customWidth="1" max="14" min="14" style="2" width="18.28515625"/>
     <col customWidth="1" max="15" min="15" style="2" width="12"/>
-    <col customWidth="1" max="16" min="16" style="2" width="17.33203125"/>
-    <col customWidth="1" max="17" min="17" style="2" width="16.44140625"/>
+    <col customWidth="1" max="16" min="16" style="2" width="17.28515625"/>
+    <col customWidth="1" max="17" min="17" style="2" width="16.42578125"/>
     <col customWidth="1" max="18" min="18" style="2" width="17"/>
-    <col customWidth="1" max="19" min="19" style="2" width="9.44140625"/>
-    <col customWidth="1" max="20" min="20" style="2" width="27.44140625"/>
-    <col customWidth="1" max="21" min="21" style="2" width="7.88671875"/>
-    <col customWidth="1" max="22" min="22" style="2" width="13.5546875"/>
+    <col customWidth="1" max="19" min="19" style="2" width="9.42578125"/>
+    <col customWidth="1" max="20" min="20" style="2" width="27.42578125"/>
+    <col customWidth="1" max="21" min="21" style="2" width="7.85546875"/>
+    <col customWidth="1" max="22" min="22" style="2" width="13.5703125"/>
     <col customWidth="1" max="23" min="23" style="2" width="46"/>
-    <col customWidth="1" max="1024" min="24" style="2" width="8.6640625"/>
+    <col customWidth="1" max="1024" min="24" style="2" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1153,7 +1159,7 @@
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="409.6" r="16" s="2">
+    <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
@@ -1341,113 +1347,9 @@
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" s="8" t="inlineStr">
-        <is>
-          <t>2004 – 15
-2003 - 16
-2002 - 17
-2001 - 18
-2000 - 19
-1999 - 20
-1998 - 21
-1997 - 22
-1996 - 23
-1995 - 24
-1994 - 25
-1993 - 26
-1992 – 27
-1991 - 28
-1990 - 29
-1989 - 30
-1988 - 31
-1987 - 32
-1986 - 33
-1985 - 34
-1984 - 35
-1983 - 36
-1982 - 37
-1981 - 38
-1980 - 39
-1979 - 40
-1978 - 41
-1977 - 42
-1976 - 43
-1975 - 44
-1974 - 45
-1973 - 46
-1972 - 47
-1971 - 48
-1970 - 49
-1969 - 50
-1968 - 51
-1967 - 52
-1966 - 53
-1965 - 54
-1964 - 55
-1963 - 56
-1962 - 57
-1961 - 58
-1960 - 59
-1959 - 60
-1958 - 61
-1957 - 62
-1956 - 63
-1955 - 64
-1954 - 65
-1953 - 66
-1952 - 67
-1951 - 68
-1950 - 69
-1949 - 70
-1948 - 71
-1947 - 72
-1946 - 73
-1945 - 74
-1944 - 75
-1943 - 76
-1942 - 77
-1941 - 78
-1940 - 79
-1939 - 80
-1938 - 81
-1937 - 82
-1936 - 83
-1935 - 84
-1934 - 85
-1933 - 86
-1932 - 87
-1931 - 88
-1930 - 89
-1929 - 90
-1928 - 91
-1927 - 92
-1926 - 93
-1925 - 94
-1924 - 95
-1923 - 96
-1922 - 97
-1921 - 98
-1920 - 99
-1919 - 100
-1918 - 101
-1917 - 102
-1916 - 103
-1915 - 104
-1914 - 105
-1913 - 106
-1912 - 107
-1911 - 108
-1910 - 109
-1909 - 110
-1908 - 111
-1907 - 112
-1906 - 113
-1905 - 114
-1904 - 115
-1903 - 116
-1902 - 117
-1901 - 118
-1900 - 119</t>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>2004 – 15&lt;br&gt;2003 - 16&lt;br&gt;2002 - 17&lt;br&gt;2001 - 18&lt;br&gt;2000 - 19&lt;br&gt;1999 - 20&lt;br&gt;1998 - 21&lt;br&gt;1997 - 22&lt;br&gt;1996 - 23&lt;br&gt;1995 - 24&lt;br&gt;1994 - 25&lt;br&gt;1993 - 26&lt;br&gt;1992 – 27&lt;br&gt;1991 - 28&lt;br&gt;1990 - 29&lt;br&gt;1989 - 30&lt;br&gt;1988 - 31&lt;br&gt;1987 - 32&lt;br&gt;1986 - 33&lt;br&gt;1985 - 34&lt;br&gt;1984 - 35&lt;br&gt;1983 - 36&lt;br&gt;1982 - 37&lt;br&gt;1981 - 38&lt;br&gt;1980 - 39&lt;br&gt;1979 - 40&lt;br&gt;1978 - 41&lt;br&gt;1977 - 42&lt;br&gt;1976 - 43&lt;br&gt;1975 - 44&lt;br&gt;1974 - 45&lt;br&gt;1973 - 46&lt;br&gt;1972 - 47&lt;br&gt;1971 - 48&lt;br&gt;1970 - 49&lt;br&gt;1969 - 50&lt;br&gt;1968 - 51&lt;br&gt;1967 - 52&lt;br&gt;1966 - 53&lt;br&gt;1965 - 54&lt;br&gt;1964 - 55&lt;br&gt;1963 - 56&lt;br&gt;1962 - 57&lt;br&gt;1961 - 58&lt;br&gt;1960 - 59&lt;br&gt;1959 - 60&lt;br&gt;1958 - 61&lt;br&gt;1957 - 62&lt;br&gt;1956 - 63&lt;br&gt;1955 - 64&lt;br&gt;1954 - 65&lt;br&gt;1953 - 66&lt;br&gt;1952 - 67&lt;br&gt;1951 - 68&lt;br&gt;1950 - 69&lt;br&gt;1949 - 70&lt;br&gt;1948 - 71&lt;br&gt;1947 - 72&lt;br&gt;1946 - 73&lt;br&gt;1945 - 74&lt;br&gt;1944 - 75&lt;br&gt;1943 - 76&lt;br&gt;1942 - 77&lt;br&gt;1941 - 78&lt;br&gt;1940 - 79&lt;br&gt;1939 - 80&lt;br&gt;1938 - 81&lt;br&gt;1937 - 82&lt;br&gt;1936 - 83&lt;br&gt;1935 - 84&lt;br&gt;1934 - 85&lt;br&gt;1933 - 86&lt;br&gt;1932 - 87&lt;br&gt;1931 - 88&lt;br&gt;1930 - 89&lt;br&gt;1929 - 90&lt;br&gt;1928 - 91&lt;br&gt;1927 - 92&lt;br&gt;1926 - 93&lt;br&gt;1925 - 94&lt;br&gt;1924 - 95&lt;br&gt;1923 - 96&lt;br&gt;1922 - 97&lt;br&gt;1921 - 98&lt;br&gt;1920 - 99&lt;br&gt;1919 - 100&lt;br&gt;1918 - 101&lt;br&gt;1917 - 102&lt;br&gt;1916 - 103&lt;br&gt;1915 - 104&lt;br&gt;1914 - 105&lt;br&gt;1913 - 106&lt;br&gt;1912 - 107&lt;br&gt;1911 - 108&lt;br&gt;1910 - 109&lt;br&gt;1909 - 110&lt;br&gt;1908 - 111&lt;br&gt;1907 - 112&lt;br&gt;1906 - 113&lt;br&gt;1905 - 114&lt;br&gt;1904 - 115&lt;br&gt;1903 - 116&lt;br&gt;1902 - 117&lt;br&gt;1901 - 118&lt;br&gt;1900 - 119</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1597,7 +1499,7 @@
       <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.7" r="24" s="2">
+    <row customHeight="1" ht="17.65" r="24" s="2">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
@@ -1651,7 +1553,7 @@
       <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.7" r="25" s="2">
+    <row customHeight="1" ht="17.65" r="25" s="2">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
@@ -1685,7 +1587,7 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.7" r="26" s="2">
+    <row customHeight="1" ht="17.65" r="26" s="2">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
@@ -1735,7 +1637,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.7" r="27" s="2">
+    <row customHeight="1" ht="17.65" r="27" s="2">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
@@ -5297,20 +5199,20 @@
       <selection activeCell="B10" activeCellId="1" sqref="A32:XFD32 B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="30.88671875"/>
+    <col customWidth="1" max="1" min="1" style="2" width="30.85546875"/>
     <col customWidth="1" max="2" min="2" style="2" width="20"/>
-    <col customWidth="1" max="1025" min="3" style="2" width="8.6640625"/>
+    <col customWidth="1" max="1025" min="3" style="2" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>setting_name</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>value</t>
         </is>
@@ -5322,46 +5224,46 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>table_id</t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B2" s="9" t="inlineStr">
         <is>
           <t>person</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>form_id</t>
         </is>
       </c>
-      <c r="B3" s="10" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
           <t>person</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>form_version</t>
         </is>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>survey</t>
         </is>
       </c>
-      <c r="C5" s="10" t="inlineStr">
+      <c r="C5" s="9" t="inlineStr">
         <is>
           <t>New Person</t>
         </is>
@@ -5393,10 +5295,10 @@
       <selection activeCell="G72" activeCellId="1" sqref="A32:XFD32 G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="43.5546875"/>
-    <col customWidth="1" max="1025" min="2" style="2" width="8.6640625"/>
+    <col customWidth="1" max="1" min="1" style="2" width="43.5703125"/>
+    <col customWidth="1" max="1025" min="2" style="2" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5849,23 +5751,23 @@
       <selection activeCell="C35" activeCellId="1" sqref="A32:XFD32 C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.6640625"/>
+    <col customWidth="1" max="1025" min="1" style="2" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>choice_list_name</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>data_value</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>display.title.text</t>
         </is>

</xml_diff>

<commit_message>
Update form-convert.exe, add rodent form
</commit_message>
<xml_diff>
--- a/app/designerFiles/app/config/tables/person/forms/person/person.xlsx
+++ b/app/designerFiles/app/config/tables/person/forms/person/person.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -28,7 +28,7 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
       <color rgb="FFFFFFFF"/>
       <sz val="10"/>
     </font>
@@ -41,7 +41,7 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
@@ -50,6 +50,19 @@
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF3C4043"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -78,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -86,9 +99,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -100,6 +110,9 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -409,38 +422,30 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF107"/>
+  <dimension ref="A1:AF74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="71" zoomScaleNormal="71">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="69" zoomScaleNormal="90">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="6.7109375"/>
-    <col customWidth="1" max="2" min="2" style="2" width="8.7109375"/>
-    <col customWidth="1" max="3" min="3" style="2" width="10.42578125"/>
-    <col customWidth="1" max="4" min="4" style="2" width="8.7109375"/>
-    <col customWidth="1" max="5" min="5" style="2" width="26.42578125"/>
-    <col customWidth="1" max="6" min="6" style="2" width="19.5703125"/>
-    <col customWidth="1" max="7" min="7" style="2" width="21.7109375"/>
-    <col customWidth="1" max="8" min="8" style="2" width="79.28515625"/>
-    <col customWidth="1" max="9" min="9" style="2" width="57.140625"/>
-    <col customWidth="1" max="10" min="10" style="2" width="13"/>
-    <col customWidth="1" max="11" min="11" style="2" width="20.7109375"/>
-    <col customWidth="1" max="12" min="12" style="2" width="14.140625"/>
-    <col customWidth="1" max="13" min="13" style="2" width="17.85546875"/>
-    <col customWidth="1" max="14" min="14" style="2" width="18.28515625"/>
-    <col customWidth="1" max="15" min="15" style="2" width="12"/>
-    <col customWidth="1" max="16" min="16" style="2" width="17.28515625"/>
-    <col customWidth="1" max="17" min="17" style="2" width="16.42578125"/>
-    <col customWidth="1" max="18" min="18" style="2" width="17"/>
-    <col customWidth="1" max="19" min="19" style="2" width="9.42578125"/>
-    <col customWidth="1" max="20" min="20" style="2" width="27.42578125"/>
-    <col customWidth="1" max="21" min="21" style="2" width="7.85546875"/>
-    <col customWidth="1" max="22" min="22" style="2" width="13.5703125"/>
-    <col customWidth="1" max="23" min="23" style="2" width="46"/>
-    <col customWidth="1" max="1024" min="24" style="2" width="8.7109375"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="12" width="34"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="12" width="14.7109375"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="12" width="9.7109375"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="12" width="14.7109375"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="12" width="32"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="12" width="12.28515625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="12" width="20.140625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="12" width="13.140625"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="12" width="17.28515625"/>
+    <col bestFit="1" customWidth="1" max="14" min="14" style="12" width="17.7109375"/>
+    <col bestFit="1" customWidth="1" max="15" min="15" style="12" width="11.42578125"/>
+    <col bestFit="1" customWidth="1" max="16" min="16" style="12" width="16.28515625"/>
+    <col bestFit="1" customWidth="1" max="17" min="17" style="12" width="15.42578125"/>
+    <col bestFit="1" customWidth="1" max="18" min="18" style="12" width="16"/>
+    <col bestFit="1" customWidth="1" max="19" min="19" style="12" width="8.7109375"/>
+    <col bestFit="1" customWidth="1" max="20" min="20" style="12" width="26.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -597,31 +602,31 @@
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
-      <c r="AF2" s="4" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>consent</t>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">select_one </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>consent</t>
+          <t>select_one</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1. I'd like to ask you questions in order to help us conduct research in hopes to improve healthcare for Lassa fever. Redeemer University, the University of Cambridge, and our partners may have access to this information, including your current location, and potentially voice recording. If you accept, you may withdraw your permission at any time and ask for your data to be erased. Choosing to not participate will in no way affect the care and treatment you will receive. Are happy to participate?</t>
+          <t>1. What is the name of the interviewer?</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -670,7 +675,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'consent',data('consent')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'interviewer_name',data('interviewer_name')]]))</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -698,10 +703,18 @@
       <c r="AF4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t>selected(data('interviewer_name'), 'Other')</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -732,36 +745,40 @@
       <c r="AF5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>if</t>
-        </is>
-      </c>
-      <c r="B6" s="6" t="inlineStr"/>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
-          <t>data('consent') == 'Yes'</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr"/>
-      <c r="F6" s="6" t="inlineStr"/>
-      <c r="G6" s="6" t="inlineStr"/>
-      <c r="H6" s="6" t="inlineStr"/>
-      <c r="I6" s="6" t="inlineStr"/>
-      <c r="J6" s="6" t="inlineStr"/>
-      <c r="K6" s="6" t="inlineStr"/>
-      <c r="L6" s="6" t="inlineStr"/>
-      <c r="M6" s="6" t="inlineStr"/>
-      <c r="N6" s="6" t="inlineStr"/>
-      <c r="O6" s="6" t="inlineStr"/>
-      <c r="P6" s="6" t="inlineStr"/>
-      <c r="Q6" s="6" t="inlineStr"/>
-      <c r="R6" s="6" t="inlineStr"/>
-      <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" s="6" t="inlineStr"/>
-      <c r="U6" s="6" t="inlineStr"/>
-      <c r="V6" s="6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" s="8" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>interviewer_name_other</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>What is the name of the interviewer?</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
@@ -773,20 +790,28 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
     </row>
-    <row r="7" s="2">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>begin screen</t>
-        </is>
-      </c>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'interviewer_name_other',data('interviewer_name_other')]]))</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -812,26 +837,18 @@
       <c r="AF7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>end if</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>3. What is your first name?</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -844,11 +861,7 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" s="6" t="inlineStr">
-        <is>
-          <t>data('consent') == 'Yes'</t>
-        </is>
-      </c>
+      <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
@@ -866,10 +879,26 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>consent</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">select_one </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>consent</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2. I'd like to ask you questions in order to help us conduct research in hopes to improve healthcare for Lassa fever. Redeemer University, the University of Cambridge, and our partners may have access to this information, including your current location. .  Note that you may withdraw your permission at any time and ask for your data to be erased. Choosing to not participate will in no way affect the care and treatment you will receive. Are you happy to participate?</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -882,7 +911,9 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="n">
+        <v>1</v>
+      </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -903,27 +934,23 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>other_name</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>4. What is your other name?</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
+          <t>log</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'consent',data('consent')]]))</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Skip if none.</t>
-        </is>
-      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -946,28 +973,36 @@
       <c r="AF10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr"/>
+      <c r="F11" s="5" t="inlineStr"/>
+      <c r="G11" s="5" t="inlineStr"/>
+      <c r="H11" s="5" t="inlineStr"/>
+      <c r="I11" s="5" t="inlineStr"/>
+      <c r="J11" s="5" t="inlineStr"/>
+      <c r="K11" s="5" t="inlineStr"/>
+      <c r="L11" s="5" t="inlineStr"/>
+      <c r="M11" s="5" t="inlineStr"/>
+      <c r="N11" s="5" t="inlineStr"/>
+      <c r="O11" s="5" t="inlineStr"/>
+      <c r="P11" s="5" t="inlineStr"/>
+      <c r="Q11" s="5" t="inlineStr"/>
+      <c r="R11" s="5" t="inlineStr"/>
+      <c r="S11" s="5" t="inlineStr"/>
+      <c r="T11" s="5" t="inlineStr"/>
+      <c r="U11" s="5" t="inlineStr"/>
+      <c r="V11" s="5" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
@@ -980,26 +1015,18 @@
       <c r="AF11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>begin screen</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>surname</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2. What is your surname?</t>
-        </is>
-      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -1012,11 +1039,7 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" s="6" t="inlineStr">
-        <is>
-          <t>data('consent') == 'Yes'</t>
-        </is>
-      </c>
+      <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
@@ -1030,18 +1053,26 @@
       <c r="AF12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>end screen</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>3. What is your first name?</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1054,7 +1085,11 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" s="5" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
@@ -1067,28 +1102,16 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="10.5" r="14" s="2">
+    <row r="14">
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'surname',data('surname')]]))</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
@@ -1113,7 +1136,7 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="10.5" r="15" s="2">
+    <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
@@ -1121,23 +1144,27 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>assign</t>
+          <t>text</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'other_name',data('other_name')]]))</t>
-        </is>
-      </c>
+          <t>other_name</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>4. What is your other name?</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Skip if none.</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
@@ -1165,22 +1192,10 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'first_name',data('first_name')]]))</t>
-        </is>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1206,18 +1221,26 @@
       <c r="AF16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>begin screen</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>surname</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>5. What is your surname?</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1230,7 +1253,11 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" s="5" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
@@ -1244,26 +1271,18 @@
       <c r="AF17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>end screen</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>5. Age at last birthday (in years)</t>
-        </is>
-      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -1274,21 +1293,9 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>data('age') &lt;= 150 &amp;&amp; data('age') &gt;= 0</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>Enter age in years:</t>
-        </is>
-      </c>
-      <c r="U18" s="6" t="inlineStr">
-        <is>
-          <t>data('consent') == 'Yes'</t>
-        </is>
-      </c>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
@@ -1307,10 +1314,22 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'surname',data('surname')]]))</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1322,7 +1341,7 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" s="6" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
@@ -1343,16 +1362,20 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" s="10" t="inlineStr">
-        <is>
-          <t>2004 – 15&lt;br&gt;2003 - 16&lt;br&gt;2002 - 17&lt;br&gt;2001 - 18&lt;br&gt;2000 - 19&lt;br&gt;1999 - 20&lt;br&gt;1998 - 21&lt;br&gt;1997 - 22&lt;br&gt;1996 - 23&lt;br&gt;1995 - 24&lt;br&gt;1994 - 25&lt;br&gt;1993 - 26&lt;br&gt;1992 – 27&lt;br&gt;1991 - 28&lt;br&gt;1990 - 29&lt;br&gt;1989 - 30&lt;br&gt;1988 - 31&lt;br&gt;1987 - 32&lt;br&gt;1986 - 33&lt;br&gt;1985 - 34&lt;br&gt;1984 - 35&lt;br&gt;1983 - 36&lt;br&gt;1982 - 37&lt;br&gt;1981 - 38&lt;br&gt;1980 - 39&lt;br&gt;1979 - 40&lt;br&gt;1978 - 41&lt;br&gt;1977 - 42&lt;br&gt;1976 - 43&lt;br&gt;1975 - 44&lt;br&gt;1974 - 45&lt;br&gt;1973 - 46&lt;br&gt;1972 - 47&lt;br&gt;1971 - 48&lt;br&gt;1970 - 49&lt;br&gt;1969 - 50&lt;br&gt;1968 - 51&lt;br&gt;1967 - 52&lt;br&gt;1966 - 53&lt;br&gt;1965 - 54&lt;br&gt;1964 - 55&lt;br&gt;1963 - 56&lt;br&gt;1962 - 57&lt;br&gt;1961 - 58&lt;br&gt;1960 - 59&lt;br&gt;1959 - 60&lt;br&gt;1958 - 61&lt;br&gt;1957 - 62&lt;br&gt;1956 - 63&lt;br&gt;1955 - 64&lt;br&gt;1954 - 65&lt;br&gt;1953 - 66&lt;br&gt;1952 - 67&lt;br&gt;1951 - 68&lt;br&gt;1950 - 69&lt;br&gt;1949 - 70&lt;br&gt;1948 - 71&lt;br&gt;1947 - 72&lt;br&gt;1946 - 73&lt;br&gt;1945 - 74&lt;br&gt;1944 - 75&lt;br&gt;1943 - 76&lt;br&gt;1942 - 77&lt;br&gt;1941 - 78&lt;br&gt;1940 - 79&lt;br&gt;1939 - 80&lt;br&gt;1938 - 81&lt;br&gt;1937 - 82&lt;br&gt;1936 - 83&lt;br&gt;1935 - 84&lt;br&gt;1934 - 85&lt;br&gt;1933 - 86&lt;br&gt;1932 - 87&lt;br&gt;1931 - 88&lt;br&gt;1930 - 89&lt;br&gt;1929 - 90&lt;br&gt;1928 - 91&lt;br&gt;1927 - 92&lt;br&gt;1926 - 93&lt;br&gt;1925 - 94&lt;br&gt;1924 - 95&lt;br&gt;1923 - 96&lt;br&gt;1922 - 97&lt;br&gt;1921 - 98&lt;br&gt;1920 - 99&lt;br&gt;1919 - 100&lt;br&gt;1918 - 101&lt;br&gt;1917 - 102&lt;br&gt;1916 - 103&lt;br&gt;1915 - 104&lt;br&gt;1914 - 105&lt;br&gt;1913 - 106&lt;br&gt;1912 - 107&lt;br&gt;1911 - 108&lt;br&gt;1910 - 109&lt;br&gt;1909 - 110&lt;br&gt;1908 - 111&lt;br&gt;1907 - 112&lt;br&gt;1906 - 113&lt;br&gt;1905 - 114&lt;br&gt;1904 - 115&lt;br&gt;1903 - 116&lt;br&gt;1902 - 117&lt;br&gt;1901 - 118&lt;br&gt;1900 - 119</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr"/>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'other_name',data('other_name')]]))</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1378,19 +1401,27 @@
       <c r="AF20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>end screen</t>
-        </is>
-      </c>
+      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'first_name',data('first_name')]]))</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1416,27 +1447,19 @@
       <c r="AF21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>begin screen</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'age',data('age')]]))</t>
-        </is>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -1462,18 +1485,26 @@
       <c r="AF22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>begin screen</t>
-        </is>
-      </c>
+      <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>6. Age at last birthday (in years)</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -1484,9 +1515,21 @@
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>data('age') &lt;= 150 &amp;&amp; data('age') &gt;= 0</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Enter age in years:</t>
+        </is>
+      </c>
+      <c r="U23" s="5" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
@@ -1499,31 +1542,15 @@
       <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.65" r="24" s="2">
+    <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>gender</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>select_one</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>gender</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>6. Gender</t>
-        </is>
-      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -1536,11 +1563,7 @@
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" s="6" t="inlineStr">
-        <is>
-          <t>data('consent') == 'Yes'</t>
-        </is>
-      </c>
+      <c r="U24" s="5" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
@@ -1553,15 +1576,23 @@
       <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.65" r="25" s="2">
+    <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" s="9" t="inlineStr">
+        <is>
+          <t>2004 – 15&lt;br&gt;2003 - 16&lt;br&gt;2002 - 17&lt;br&gt;2001 - 18&lt;br&gt;2000 - 19&lt;br&gt;1999 - 20&lt;br&gt;1998 - 21&lt;br&gt;1997 - 22&lt;br&gt;1996 - 23&lt;br&gt;1995 - 24&lt;br&gt;1994 - 25&lt;br&gt;1993 - 26&lt;br&gt;1992 – 27&lt;br&gt;1991 - 28&lt;br&gt;1990 - 29&lt;br&gt;1989 - 30&lt;br&gt;1988 - 31&lt;br&gt;1987 - 32&lt;br&gt;1986 - 33&lt;br&gt;1985 - 34&lt;br&gt;1984 - 35&lt;br&gt;1983 - 36&lt;br&gt;1982 - 37&lt;br&gt;1981 - 38&lt;br&gt;1980 - 39&lt;br&gt;1979 - 40&lt;br&gt;1978 - 41&lt;br&gt;1977 - 42&lt;br&gt;1976 - 43&lt;br&gt;1975 - 44&lt;br&gt;1974 - 45&lt;br&gt;1973 - 46&lt;br&gt;1972 - 47&lt;br&gt;1971 - 48&lt;br&gt;1970 - 49&lt;br&gt;1969 - 50&lt;br&gt;1968 - 51&lt;br&gt;1967 - 52&lt;br&gt;1966 - 53&lt;br&gt;1965 - 54&lt;br&gt;1964 - 55&lt;br&gt;1963 - 56&lt;br&gt;1962 - 57&lt;br&gt;1961 - 58&lt;br&gt;1960 - 59&lt;br&gt;1959 - 60&lt;br&gt;1958 - 61&lt;br&gt;1957 - 62&lt;br&gt;1956 - 63&lt;br&gt;1955 - 64&lt;br&gt;1954 - 65&lt;br&gt;1953 - 66&lt;br&gt;1952 - 67&lt;br&gt;1951 - 68&lt;br&gt;1950 - 69&lt;br&gt;1949 - 70&lt;br&gt;1948 - 71&lt;br&gt;1947 - 72&lt;br&gt;1946 - 73&lt;br&gt;1945 - 74&lt;br&gt;1944 - 75&lt;br&gt;1943 - 76&lt;br&gt;1942 - 77&lt;br&gt;1941 - 78&lt;br&gt;1940 - 79&lt;br&gt;1939 - 80&lt;br&gt;1938 - 81&lt;br&gt;1937 - 82&lt;br&gt;1936 - 83&lt;br&gt;1935 - 84&lt;br&gt;1934 - 85&lt;br&gt;1933 - 86&lt;br&gt;1932 - 87&lt;br&gt;1931 - 88&lt;br&gt;1930 - 89&lt;br&gt;1929 - 90&lt;br&gt;1928 - 91&lt;br&gt;1927 - 92&lt;br&gt;1926 - 93&lt;br&gt;1925 - 94&lt;br&gt;1924 - 95&lt;br&gt;1923 - 96&lt;br&gt;1922 - 97&lt;br&gt;1921 - 98&lt;br&gt;1920 - 99&lt;br&gt;1919 - 100&lt;br&gt;1918 - 101&lt;br&gt;1917 - 102&lt;br&gt;1916 - 103&lt;br&gt;1915 - 104&lt;br&gt;1914 - 105&lt;br&gt;1913 - 106&lt;br&gt;1912 - 107&lt;br&gt;1911 - 108&lt;br&gt;1910 - 109&lt;br&gt;1909 - 110&lt;br&gt;1908 - 111&lt;br&gt;1907 - 112&lt;br&gt;1906 - 113&lt;br&gt;1905 - 114&lt;br&gt;1904 - 115&lt;br&gt;1903 - 116&lt;br&gt;1902 - 117&lt;br&gt;1901 - 118&lt;br&gt;1900 - 119</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -1587,28 +1618,20 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.65" r="26" s="2">
-      <c r="A26" t="inlineStr"/>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>end screen</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>registration_date</t>
-        </is>
-      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>odkCommon.toOdkTimeStampFromDate(new Date())</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -1622,11 +1645,7 @@
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>Default registration date to today</t>
-        </is>
-      </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr"/>
@@ -1637,7 +1656,7 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="17.65" r="27" s="2">
+    <row customHeight="1" ht="15.75" r="27" s="12">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
@@ -1645,27 +1664,23 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>registration_date</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>7. Registration date</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
+          <t>log</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'age',data('age')]]))</t>
+        </is>
+      </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Today's date</t>
-        </is>
-      </c>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
@@ -1674,11 +1689,7 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>data('consent') == 'Yes'</t>
-        </is>
-      </c>
+      <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
@@ -1691,8 +1702,12 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="12.75" r="28" s="2">
-      <c r="A28" t="inlineStr"/>
+    <row customHeight="1" ht="15.75" r="28" s="12">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>begin screen</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
@@ -1732,32 +1747,28 @@
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>photo_consent</t>
+          <t>gender</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve">select_one </t>
+          <t>select_one</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>photo_consent</t>
+          <t>gender</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>46. May I take your photo?</t>
+          <t>7. Gender</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>It's not necessary.</t>
-        </is>
-      </c>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
@@ -1766,7 +1777,11 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
+      <c r="U29" s="5" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
@@ -1779,19 +1794,11 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="12.75" r="30" s="2">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>if</t>
-        </is>
-      </c>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>data('photo_consent') == 'Yes'</t>
-        </is>
-      </c>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -1821,25 +1828,29 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="12.75" r="31" s="2">
+    <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>marital_status</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>image</t>
+          <t>select_one</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>photo</t>
+          <t>marital_status</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>47. [Take picture of full face]</t>
+          <t>8. Marital status</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -1867,10 +1878,10 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr"/>
     </row>
-    <row customHeight="1" ht="12.75" r="32" s="2">
+    <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>end if</t>
+          <t>end screen</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1911,10 +1922,22 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'marital_status',data('marital_status')]]))</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -1945,10 +1968,22 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'gender',data('gender')]]))</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
@@ -1976,7 +2011,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>end screen</t>
+          <t>begin screen</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -2016,23 +2051,27 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'photo',data('photo')]]))</t>
-        </is>
-      </c>
+      <c r="E36" s="10" t="inlineStr">
+        <is>
+          <t>p_lassa</t>
+        </is>
+      </c>
+      <c r="F36" s="10" t="inlineStr">
+        <is>
+          <t>select_one</t>
+        </is>
+      </c>
+      <c r="G36" s="10" t="inlineStr">
+        <is>
+          <t>p_lassa</t>
+        </is>
+      </c>
+      <c r="H36" s="10" t="inlineStr">
+        <is>
+          <t>9. Have you ever been diagnosed with Lassa fever at a hospital?</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2044,7 +2083,11 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
@@ -2062,23 +2105,11 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'photo_consent',data('photo_consent')]]))</t>
-        </is>
-      </c>
+      <c r="E37" s="10" t="inlineStr"/>
+      <c r="F37" s="10" t="inlineStr"/>
+      <c r="G37" s="10" t="inlineStr"/>
+      <c r="H37" s="10" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2108,23 +2139,27 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>cohort</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>assign</t>
+          <t>select_one</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'registration_date',data('registration_date')]]))</t>
-        </is>
-      </c>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>10. What cohort does this person belong to?</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2136,7 +2171,11 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V38" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
@@ -2150,27 +2189,19 @@
       <c r="AF38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>end screen</t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'registration_date',data('registration_date')]]))</t>
-        </is>
-      </c>
+      <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2214,7 +2245,7 @@
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'gender',data('gender')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'cohort',data('cohort')]]))</t>
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
@@ -2242,19 +2273,27 @@
       <c r="AF40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>end if</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>log</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'p_lassa',data('p_lassa')]]))</t>
+        </is>
+      </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2280,7 +2319,11 @@
       <c r="AF41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>begin screen</t>
+        </is>
+      </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
@@ -2319,9 +2362,21 @@
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>phone_number</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>1. Phone number</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
@@ -2387,10 +2442,22 @@
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>assign</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>registration_date</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>odkCommon.toOdkTimeStampFromDate(new Date())</t>
+        </is>
+      </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2404,7 +2471,11 @@
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>Default registration date to today</t>
+        </is>
+      </c>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
       <c r="Z45" t="inlineStr"/>
@@ -2416,24 +2487,34 @@
       <c r="AF45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>if</t>
-        </is>
-      </c>
+      <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>registration_date</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>12. Registration date</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Today's date</t>
+        </is>
+      </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
@@ -2442,7 +2523,11 @@
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>data('consent') == 'Yes'</t>
+        </is>
+      </c>
       <c r="V46" t="inlineStr"/>
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
@@ -2461,16 +2546,8 @@
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>extra_question1</t>
-        </is>
-      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
@@ -2505,20 +2582,20 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>assign</t>
+          <t>text</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question1',data('extra_question1')]]))</t>
-        </is>
-      </c>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>13. Additional notes</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -2544,21 +2621,17 @@
       <c r="AF48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>end screen</t>
+        </is>
+      </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>extra_question2</t>
-        </is>
-      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
@@ -2604,7 +2677,7 @@
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question2',data('extra_question2')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'notes',data('notes')]]))</t>
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
@@ -2639,16 +2712,20 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>extra_question3</t>
+          <t>log</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'registration_date',data('registration_date')]]))</t>
+        </is>
+      </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -2692,7 +2769,7 @@
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question3',data('extra_question3')]]))</t>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'registration_date',data('registration_date')]]))</t>
         </is>
       </c>
       <c r="J52" t="inlineStr"/>
@@ -2727,16 +2804,20 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>extra_question4</t>
+          <t>log</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'phone_number',data('phone_number')]]))</t>
+        </is>
+      </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
@@ -2762,27 +2843,19 @@
       <c r="AF53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>end if</t>
+        </is>
+      </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question4',data('extra_question4')]]))</t>
-        </is>
-      </c>
+      <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
@@ -2815,16 +2888,20 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>extra_question5</t>
+          <t>log_0</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>data('log').substring(0,60000) == '' ? ' ' : data('log').substring(0,60000)</t>
+        </is>
+      </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
@@ -2862,13 +2939,13 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_1</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question5',data('extra_question5')]]))</t>
+          <t>data('log').substring(60000,120000) == '' ? ' ' : data('log').substring(60000,120000)</t>
         </is>
       </c>
       <c r="J56" t="inlineStr"/>
@@ -2903,16 +2980,20 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>extra_question6</t>
+          <t>log_2</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>data('log').substring(120000,180000) == '' ? ' ' : data('log').substring(120000,180000)</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>
@@ -2950,13 +3031,13 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_3</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question6',data('extra_question6')]]))</t>
+          <t>data('log').substring(180000,240000) == '' ? ' ' : data('log').substring(180000,240000)</t>
         </is>
       </c>
       <c r="J58" t="inlineStr"/>
@@ -2991,16 +3072,20 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>extra_question7</t>
+          <t>log_4</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>data('log').substring(240000,300000) == '' ? ' ' : data('log').substring(240000,300000)</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
@@ -3038,13 +3123,13 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_5</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question7',data('extra_question7')]]))</t>
+          <t>data('log').substring(300000,360000) == '' ? ' ' : data('log').substring(300000,360000)</t>
         </is>
       </c>
       <c r="J60" t="inlineStr"/>
@@ -3079,16 +3164,20 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>extra_question8</t>
+          <t>log_6</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>data('log').substring(360000,420000) == '' ? ' ' : data('log').substring(360000,420000)</t>
+        </is>
+      </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
@@ -3126,13 +3215,13 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_7</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question8',data('extra_question8')]]))</t>
+          <t>data('log').substring(420000,480000) == '' ? ' ' : data('log').substring(420000,480000)</t>
         </is>
       </c>
       <c r="J62" t="inlineStr"/>
@@ -3167,16 +3256,20 @@
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>extra_question9</t>
+          <t>log_8</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>data('log').substring(480000,540000) == '' ? ' ' : data('log').substring(480000,540000)</t>
+        </is>
+      </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
@@ -3214,13 +3307,13 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_9</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question9',data('extra_question9')]]))</t>
+          <t>data('log').substring(540000,600000) == '' ? ' ' : data('log').substring(540000,600000)</t>
         </is>
       </c>
       <c r="J64" t="inlineStr"/>
@@ -3255,16 +3348,20 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>extra_question10</t>
+          <t>log_10</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>data('log').substring(600000,660000) == '' ? ' ' : data('log').substring(600000,660000)</t>
+        </is>
+      </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
@@ -3302,13 +3399,13 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_11</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question10',data('extra_question10')]]))</t>
+          <t>data('log').substring(660000,720000) == '' ? ' ' : data('log').substring(660000,720000)</t>
         </is>
       </c>
       <c r="J66" t="inlineStr"/>
@@ -3343,16 +3440,20 @@
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>extra_question11</t>
+          <t>log_12</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>data('log').substring(720000,780000) == '' ? ' ' : data('log').substring(720000,780000)</t>
+        </is>
+      </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr"/>
@@ -3390,13 +3491,13 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_13</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question11',data('extra_question11')]]))</t>
+          <t>data('log').substring(780000,840000) == '' ? ' ' : data('log').substring(780000,840000)</t>
         </is>
       </c>
       <c r="J68" t="inlineStr"/>
@@ -3431,16 +3532,20 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>extra_question12</t>
+          <t>log_14</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>data('log').substring(840000,900000) == '' ? ' ' : data('log').substring(840000,900000)</t>
+        </is>
+      </c>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr"/>
@@ -3478,13 +3583,13 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_15</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question12',data('extra_question12')]]))</t>
+          <t>data('log').substring(900000,960000) == '' ? ' ' : data('log').substring(900000,960000)</t>
         </is>
       </c>
       <c r="J70" t="inlineStr"/>
@@ -3519,16 +3624,20 @@
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>extra_question13</t>
+          <t>log_16</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>data('log').substring(960000,1020000) == '' ? ' ' : data('log').substring(960000,1020000)</t>
+        </is>
+      </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
@@ -3566,13 +3675,13 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_17</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question13',data('extra_question13')]]))</t>
+          <t>data('log').substring(1020000,1080000) == '' ? ' ' : data('log').substring(1020000,1080000)</t>
         </is>
       </c>
       <c r="J72" t="inlineStr"/>
@@ -3607,16 +3716,20 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>assign</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>extra_question14</t>
+          <t>log_18</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>data('log').substring(1080000,1140000) == '' ? ' ' : data('log').substring(1080000,1140000)</t>
+        </is>
+      </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
@@ -3654,13 +3767,13 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>log</t>
+          <t>log_19</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr">
         <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question14',data('extra_question14')]]))</t>
+          <t>data('log').substring(1140000,1200000) == '' ? ' ' : data('log').substring(1140000,1200000)</t>
         </is>
       </c>
       <c r="J74" t="inlineStr"/>
@@ -3687,1503 +3800,8 @@
       <c r="AE74" t="inlineStr"/>
       <c r="AF74" t="inlineStr"/>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr"/>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>extra_question15</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
-      <c r="J75" t="inlineStr"/>
-      <c r="K75" t="inlineStr"/>
-      <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
-      <c r="N75" t="inlineStr"/>
-      <c r="O75" t="inlineStr"/>
-      <c r="P75" t="inlineStr"/>
-      <c r="Q75" t="inlineStr"/>
-      <c r="R75" t="inlineStr"/>
-      <c r="S75" t="inlineStr"/>
-      <c r="T75" t="inlineStr"/>
-      <c r="U75" t="inlineStr"/>
-      <c r="V75" t="inlineStr"/>
-      <c r="W75" t="inlineStr"/>
-      <c r="X75" t="inlineStr"/>
-      <c r="Y75" t="inlineStr"/>
-      <c r="Z75" t="inlineStr"/>
-      <c r="AA75" t="inlineStr"/>
-      <c r="AB75" t="inlineStr"/>
-      <c r="AC75" t="inlineStr"/>
-      <c r="AD75" t="inlineStr"/>
-      <c r="AE75" t="inlineStr"/>
-      <c r="AF75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr"/>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question15',data('extra_question15')]]))</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr"/>
-      <c r="K76" t="inlineStr"/>
-      <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr"/>
-      <c r="N76" t="inlineStr"/>
-      <c r="O76" t="inlineStr"/>
-      <c r="P76" t="inlineStr"/>
-      <c r="Q76" t="inlineStr"/>
-      <c r="R76" t="inlineStr"/>
-      <c r="S76" t="inlineStr"/>
-      <c r="T76" t="inlineStr"/>
-      <c r="U76" t="inlineStr"/>
-      <c r="V76" t="inlineStr"/>
-      <c r="W76" t="inlineStr"/>
-      <c r="X76" t="inlineStr"/>
-      <c r="Y76" t="inlineStr"/>
-      <c r="Z76" t="inlineStr"/>
-      <c r="AA76" t="inlineStr"/>
-      <c r="AB76" t="inlineStr"/>
-      <c r="AC76" t="inlineStr"/>
-      <c r="AD76" t="inlineStr"/>
-      <c r="AE76" t="inlineStr"/>
-      <c r="AF76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr"/>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>extra_question16</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
-      <c r="J77" t="inlineStr"/>
-      <c r="K77" t="inlineStr"/>
-      <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
-      <c r="N77" t="inlineStr"/>
-      <c r="O77" t="inlineStr"/>
-      <c r="P77" t="inlineStr"/>
-      <c r="Q77" t="inlineStr"/>
-      <c r="R77" t="inlineStr"/>
-      <c r="S77" t="inlineStr"/>
-      <c r="T77" t="inlineStr"/>
-      <c r="U77" t="inlineStr"/>
-      <c r="V77" t="inlineStr"/>
-      <c r="W77" t="inlineStr"/>
-      <c r="X77" t="inlineStr"/>
-      <c r="Y77" t="inlineStr"/>
-      <c r="Z77" t="inlineStr"/>
-      <c r="AA77" t="inlineStr"/>
-      <c r="AB77" t="inlineStr"/>
-      <c r="AC77" t="inlineStr"/>
-      <c r="AD77" t="inlineStr"/>
-      <c r="AE77" t="inlineStr"/>
-      <c r="AF77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr"/>
-      <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question16',data('extra_question16')]]))</t>
-        </is>
-      </c>
-      <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr"/>
-      <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr"/>
-      <c r="N78" t="inlineStr"/>
-      <c r="O78" t="inlineStr"/>
-      <c r="P78" t="inlineStr"/>
-      <c r="Q78" t="inlineStr"/>
-      <c r="R78" t="inlineStr"/>
-      <c r="S78" t="inlineStr"/>
-      <c r="T78" t="inlineStr"/>
-      <c r="U78" t="inlineStr"/>
-      <c r="V78" t="inlineStr"/>
-      <c r="W78" t="inlineStr"/>
-      <c r="X78" t="inlineStr"/>
-      <c r="Y78" t="inlineStr"/>
-      <c r="Z78" t="inlineStr"/>
-      <c r="AA78" t="inlineStr"/>
-      <c r="AB78" t="inlineStr"/>
-      <c r="AC78" t="inlineStr"/>
-      <c r="AD78" t="inlineStr"/>
-      <c r="AE78" t="inlineStr"/>
-      <c r="AF78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr"/>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>extra_question17</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
-      <c r="J79" t="inlineStr"/>
-      <c r="K79" t="inlineStr"/>
-      <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr"/>
-      <c r="N79" t="inlineStr"/>
-      <c r="O79" t="inlineStr"/>
-      <c r="P79" t="inlineStr"/>
-      <c r="Q79" t="inlineStr"/>
-      <c r="R79" t="inlineStr"/>
-      <c r="S79" t="inlineStr"/>
-      <c r="T79" t="inlineStr"/>
-      <c r="U79" t="inlineStr"/>
-      <c r="V79" t="inlineStr"/>
-      <c r="W79" t="inlineStr"/>
-      <c r="X79" t="inlineStr"/>
-      <c r="Y79" t="inlineStr"/>
-      <c r="Z79" t="inlineStr"/>
-      <c r="AA79" t="inlineStr"/>
-      <c r="AB79" t="inlineStr"/>
-      <c r="AC79" t="inlineStr"/>
-      <c r="AD79" t="inlineStr"/>
-      <c r="AE79" t="inlineStr"/>
-      <c r="AF79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr"/>
-      <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question17',data('extra_question17')]]))</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr"/>
-      <c r="K80" t="inlineStr"/>
-      <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr"/>
-      <c r="N80" t="inlineStr"/>
-      <c r="O80" t="inlineStr"/>
-      <c r="P80" t="inlineStr"/>
-      <c r="Q80" t="inlineStr"/>
-      <c r="R80" t="inlineStr"/>
-      <c r="S80" t="inlineStr"/>
-      <c r="T80" t="inlineStr"/>
-      <c r="U80" t="inlineStr"/>
-      <c r="V80" t="inlineStr"/>
-      <c r="W80" t="inlineStr"/>
-      <c r="X80" t="inlineStr"/>
-      <c r="Y80" t="inlineStr"/>
-      <c r="Z80" t="inlineStr"/>
-      <c r="AA80" t="inlineStr"/>
-      <c r="AB80" t="inlineStr"/>
-      <c r="AC80" t="inlineStr"/>
-      <c r="AD80" t="inlineStr"/>
-      <c r="AE80" t="inlineStr"/>
-      <c r="AF80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr"/>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>extra_question18</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr"/>
-      <c r="J81" t="inlineStr"/>
-      <c r="K81" t="inlineStr"/>
-      <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr"/>
-      <c r="N81" t="inlineStr"/>
-      <c r="O81" t="inlineStr"/>
-      <c r="P81" t="inlineStr"/>
-      <c r="Q81" t="inlineStr"/>
-      <c r="R81" t="inlineStr"/>
-      <c r="S81" t="inlineStr"/>
-      <c r="T81" t="inlineStr"/>
-      <c r="U81" t="inlineStr"/>
-      <c r="V81" t="inlineStr"/>
-      <c r="W81" t="inlineStr"/>
-      <c r="X81" t="inlineStr"/>
-      <c r="Y81" t="inlineStr"/>
-      <c r="Z81" t="inlineStr"/>
-      <c r="AA81" t="inlineStr"/>
-      <c r="AB81" t="inlineStr"/>
-      <c r="AC81" t="inlineStr"/>
-      <c r="AD81" t="inlineStr"/>
-      <c r="AE81" t="inlineStr"/>
-      <c r="AF81" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr"/>
-      <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr"/>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question18',data('extra_question18')]]))</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr"/>
-      <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr"/>
-      <c r="N82" t="inlineStr"/>
-      <c r="O82" t="inlineStr"/>
-      <c r="P82" t="inlineStr"/>
-      <c r="Q82" t="inlineStr"/>
-      <c r="R82" t="inlineStr"/>
-      <c r="S82" t="inlineStr"/>
-      <c r="T82" t="inlineStr"/>
-      <c r="U82" t="inlineStr"/>
-      <c r="V82" t="inlineStr"/>
-      <c r="W82" t="inlineStr"/>
-      <c r="X82" t="inlineStr"/>
-      <c r="Y82" t="inlineStr"/>
-      <c r="Z82" t="inlineStr"/>
-      <c r="AA82" t="inlineStr"/>
-      <c r="AB82" t="inlineStr"/>
-      <c r="AC82" t="inlineStr"/>
-      <c r="AD82" t="inlineStr"/>
-      <c r="AE82" t="inlineStr"/>
-      <c r="AF82" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr"/>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>extra_question19</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr"/>
-      <c r="K83" t="inlineStr"/>
-      <c r="L83" t="inlineStr"/>
-      <c r="M83" t="inlineStr"/>
-      <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr"/>
-      <c r="P83" t="inlineStr"/>
-      <c r="Q83" t="inlineStr"/>
-      <c r="R83" t="inlineStr"/>
-      <c r="S83" t="inlineStr"/>
-      <c r="T83" t="inlineStr"/>
-      <c r="U83" t="inlineStr"/>
-      <c r="V83" t="inlineStr"/>
-      <c r="W83" t="inlineStr"/>
-      <c r="X83" t="inlineStr"/>
-      <c r="Y83" t="inlineStr"/>
-      <c r="Z83" t="inlineStr"/>
-      <c r="AA83" t="inlineStr"/>
-      <c r="AB83" t="inlineStr"/>
-      <c r="AC83" t="inlineStr"/>
-      <c r="AD83" t="inlineStr"/>
-      <c r="AE83" t="inlineStr"/>
-      <c r="AF83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr"/>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question19',data('extra_question19')]]))</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr"/>
-      <c r="P84" t="inlineStr"/>
-      <c r="Q84" t="inlineStr"/>
-      <c r="R84" t="inlineStr"/>
-      <c r="S84" t="inlineStr"/>
-      <c r="T84" t="inlineStr"/>
-      <c r="U84" t="inlineStr"/>
-      <c r="V84" t="inlineStr"/>
-      <c r="W84" t="inlineStr"/>
-      <c r="X84" t="inlineStr"/>
-      <c r="Y84" t="inlineStr"/>
-      <c r="Z84" t="inlineStr"/>
-      <c r="AA84" t="inlineStr"/>
-      <c r="AB84" t="inlineStr"/>
-      <c r="AC84" t="inlineStr"/>
-      <c r="AD84" t="inlineStr"/>
-      <c r="AE84" t="inlineStr"/>
-      <c r="AF84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr"/>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>extra_question20</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr"/>
-      <c r="P85" t="inlineStr"/>
-      <c r="Q85" t="inlineStr"/>
-      <c r="R85" t="inlineStr"/>
-      <c r="S85" t="inlineStr"/>
-      <c r="T85" t="inlineStr"/>
-      <c r="U85" t="inlineStr"/>
-      <c r="V85" t="inlineStr"/>
-      <c r="W85" t="inlineStr"/>
-      <c r="X85" t="inlineStr"/>
-      <c r="Y85" t="inlineStr"/>
-      <c r="Z85" t="inlineStr"/>
-      <c r="AA85" t="inlineStr"/>
-      <c r="AB85" t="inlineStr"/>
-      <c r="AC85" t="inlineStr"/>
-      <c r="AD85" t="inlineStr"/>
-      <c r="AE85" t="inlineStr"/>
-      <c r="AF85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr"/>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>log</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr"/>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>JSON.stringify(((data('log')==null)?[]:JSON.parse(data('log'))).concat([[now().toUTCString(),'extra_question20',data('extra_question20')]]))</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr"/>
-      <c r="M86" t="inlineStr"/>
-      <c r="N86" t="inlineStr"/>
-      <c r="O86" t="inlineStr"/>
-      <c r="P86" t="inlineStr"/>
-      <c r="Q86" t="inlineStr"/>
-      <c r="R86" t="inlineStr"/>
-      <c r="S86" t="inlineStr"/>
-      <c r="T86" t="inlineStr"/>
-      <c r="U86" t="inlineStr"/>
-      <c r="V86" t="inlineStr"/>
-      <c r="W86" t="inlineStr"/>
-      <c r="X86" t="inlineStr"/>
-      <c r="Y86" t="inlineStr"/>
-      <c r="Z86" t="inlineStr"/>
-      <c r="AA86" t="inlineStr"/>
-      <c r="AB86" t="inlineStr"/>
-      <c r="AC86" t="inlineStr"/>
-      <c r="AD86" t="inlineStr"/>
-      <c r="AE86" t="inlineStr"/>
-      <c r="AF86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>end if</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
-      <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
-      <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
-      <c r="N87" t="inlineStr"/>
-      <c r="O87" t="inlineStr"/>
-      <c r="P87" t="inlineStr"/>
-      <c r="Q87" t="inlineStr"/>
-      <c r="R87" t="inlineStr"/>
-      <c r="S87" t="inlineStr"/>
-      <c r="T87" t="inlineStr"/>
-      <c r="U87" t="inlineStr"/>
-      <c r="V87" t="inlineStr"/>
-      <c r="W87" t="inlineStr"/>
-      <c r="X87" t="inlineStr"/>
-      <c r="Y87" t="inlineStr"/>
-      <c r="Z87" t="inlineStr"/>
-      <c r="AA87" t="inlineStr"/>
-      <c r="AB87" t="inlineStr"/>
-      <c r="AC87" t="inlineStr"/>
-      <c r="AD87" t="inlineStr"/>
-      <c r="AE87" t="inlineStr"/>
-      <c r="AF87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr"/>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>log_0</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>data('log').substring(0,60000) == '' ? ' ' : data('log').substring(0,60000)</t>
-        </is>
-      </c>
-      <c r="J88" t="inlineStr"/>
-      <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr"/>
-      <c r="Q88" t="inlineStr"/>
-      <c r="R88" t="inlineStr"/>
-      <c r="S88" t="inlineStr"/>
-      <c r="T88" t="inlineStr"/>
-      <c r="U88" t="inlineStr"/>
-      <c r="V88" t="inlineStr"/>
-      <c r="W88" t="inlineStr"/>
-      <c r="X88" t="inlineStr"/>
-      <c r="Y88" t="inlineStr"/>
-      <c r="Z88" t="inlineStr"/>
-      <c r="AA88" t="inlineStr"/>
-      <c r="AB88" t="inlineStr"/>
-      <c r="AC88" t="inlineStr"/>
-      <c r="AD88" t="inlineStr"/>
-      <c r="AE88" t="inlineStr"/>
-      <c r="AF88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr"/>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>log_1</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr"/>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>data('log').substring(60000,120000) == '' ? ' ' : data('log').substring(60000,120000)</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr"/>
-      <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr"/>
-      <c r="Q89" t="inlineStr"/>
-      <c r="R89" t="inlineStr"/>
-      <c r="S89" t="inlineStr"/>
-      <c r="T89" t="inlineStr"/>
-      <c r="U89" t="inlineStr"/>
-      <c r="V89" t="inlineStr"/>
-      <c r="W89" t="inlineStr"/>
-      <c r="X89" t="inlineStr"/>
-      <c r="Y89" t="inlineStr"/>
-      <c r="Z89" t="inlineStr"/>
-      <c r="AA89" t="inlineStr"/>
-      <c r="AB89" t="inlineStr"/>
-      <c r="AC89" t="inlineStr"/>
-      <c r="AD89" t="inlineStr"/>
-      <c r="AE89" t="inlineStr"/>
-      <c r="AF89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr"/>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>log_2</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr"/>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>data('log').substring(120000,180000) == '' ? ' ' : data('log').substring(120000,180000)</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr"/>
-      <c r="Q90" t="inlineStr"/>
-      <c r="R90" t="inlineStr"/>
-      <c r="S90" t="inlineStr"/>
-      <c r="T90" t="inlineStr"/>
-      <c r="U90" t="inlineStr"/>
-      <c r="V90" t="inlineStr"/>
-      <c r="W90" t="inlineStr"/>
-      <c r="X90" t="inlineStr"/>
-      <c r="Y90" t="inlineStr"/>
-      <c r="Z90" t="inlineStr"/>
-      <c r="AA90" t="inlineStr"/>
-      <c r="AB90" t="inlineStr"/>
-      <c r="AC90" t="inlineStr"/>
-      <c r="AD90" t="inlineStr"/>
-      <c r="AE90" t="inlineStr"/>
-      <c r="AF90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr"/>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>log_3</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>data('log').substring(180000,240000) == '' ? ' ' : data('log').substring(180000,240000)</t>
-        </is>
-      </c>
-      <c r="J91" t="inlineStr"/>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
-      <c r="O91" t="inlineStr"/>
-      <c r="P91" t="inlineStr"/>
-      <c r="Q91" t="inlineStr"/>
-      <c r="R91" t="inlineStr"/>
-      <c r="S91" t="inlineStr"/>
-      <c r="T91" t="inlineStr"/>
-      <c r="U91" t="inlineStr"/>
-      <c r="V91" t="inlineStr"/>
-      <c r="W91" t="inlineStr"/>
-      <c r="X91" t="inlineStr"/>
-      <c r="Y91" t="inlineStr"/>
-      <c r="Z91" t="inlineStr"/>
-      <c r="AA91" t="inlineStr"/>
-      <c r="AB91" t="inlineStr"/>
-      <c r="AC91" t="inlineStr"/>
-      <c r="AD91" t="inlineStr"/>
-      <c r="AE91" t="inlineStr"/>
-      <c r="AF91" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr"/>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>log_4</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>data('log').substring(240000,300000) == '' ? ' ' : data('log').substring(240000,300000)</t>
-        </is>
-      </c>
-      <c r="J92" t="inlineStr"/>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr"/>
-      <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr"/>
-      <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
-      <c r="T92" t="inlineStr"/>
-      <c r="U92" t="inlineStr"/>
-      <c r="V92" t="inlineStr"/>
-      <c r="W92" t="inlineStr"/>
-      <c r="X92" t="inlineStr"/>
-      <c r="Y92" t="inlineStr"/>
-      <c r="Z92" t="inlineStr"/>
-      <c r="AA92" t="inlineStr"/>
-      <c r="AB92" t="inlineStr"/>
-      <c r="AC92" t="inlineStr"/>
-      <c r="AD92" t="inlineStr"/>
-      <c r="AE92" t="inlineStr"/>
-      <c r="AF92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr"/>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>log_5</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>data('log').substring(300000,360000) == '' ? ' ' : data('log').substring(300000,360000)</t>
-        </is>
-      </c>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr"/>
-      <c r="P93" t="inlineStr"/>
-      <c r="Q93" t="inlineStr"/>
-      <c r="R93" t="inlineStr"/>
-      <c r="S93" t="inlineStr"/>
-      <c r="T93" t="inlineStr"/>
-      <c r="U93" t="inlineStr"/>
-      <c r="V93" t="inlineStr"/>
-      <c r="W93" t="inlineStr"/>
-      <c r="X93" t="inlineStr"/>
-      <c r="Y93" t="inlineStr"/>
-      <c r="Z93" t="inlineStr"/>
-      <c r="AA93" t="inlineStr"/>
-      <c r="AB93" t="inlineStr"/>
-      <c r="AC93" t="inlineStr"/>
-      <c r="AD93" t="inlineStr"/>
-      <c r="AE93" t="inlineStr"/>
-      <c r="AF93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr"/>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>log_6</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr"/>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>data('log').substring(360000,420000) == '' ? ' ' : data('log').substring(360000,420000)</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr"/>
-      <c r="P94" t="inlineStr"/>
-      <c r="Q94" t="inlineStr"/>
-      <c r="R94" t="inlineStr"/>
-      <c r="S94" t="inlineStr"/>
-      <c r="T94" t="inlineStr"/>
-      <c r="U94" t="inlineStr"/>
-      <c r="V94" t="inlineStr"/>
-      <c r="W94" t="inlineStr"/>
-      <c r="X94" t="inlineStr"/>
-      <c r="Y94" t="inlineStr"/>
-      <c r="Z94" t="inlineStr"/>
-      <c r="AA94" t="inlineStr"/>
-      <c r="AB94" t="inlineStr"/>
-      <c r="AC94" t="inlineStr"/>
-      <c r="AD94" t="inlineStr"/>
-      <c r="AE94" t="inlineStr"/>
-      <c r="AF94" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr"/>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>log_7</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>data('log').substring(420000,480000) == '' ? ' ' : data('log').substring(420000,480000)</t>
-        </is>
-      </c>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
-      <c r="P95" t="inlineStr"/>
-      <c r="Q95" t="inlineStr"/>
-      <c r="R95" t="inlineStr"/>
-      <c r="S95" t="inlineStr"/>
-      <c r="T95" t="inlineStr"/>
-      <c r="U95" t="inlineStr"/>
-      <c r="V95" t="inlineStr"/>
-      <c r="W95" t="inlineStr"/>
-      <c r="X95" t="inlineStr"/>
-      <c r="Y95" t="inlineStr"/>
-      <c r="Z95" t="inlineStr"/>
-      <c r="AA95" t="inlineStr"/>
-      <c r="AB95" t="inlineStr"/>
-      <c r="AC95" t="inlineStr"/>
-      <c r="AD95" t="inlineStr"/>
-      <c r="AE95" t="inlineStr"/>
-      <c r="AF95" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr"/>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>log_8</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>data('log').substring(480000,540000) == '' ? ' ' : data('log').substring(480000,540000)</t>
-        </is>
-      </c>
-      <c r="J96" t="inlineStr"/>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr"/>
-      <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr"/>
-      <c r="P96" t="inlineStr"/>
-      <c r="Q96" t="inlineStr"/>
-      <c r="R96" t="inlineStr"/>
-      <c r="S96" t="inlineStr"/>
-      <c r="T96" t="inlineStr"/>
-      <c r="U96" t="inlineStr"/>
-      <c r="V96" t="inlineStr"/>
-      <c r="W96" t="inlineStr"/>
-      <c r="X96" t="inlineStr"/>
-      <c r="Y96" t="inlineStr"/>
-      <c r="Z96" t="inlineStr"/>
-      <c r="AA96" t="inlineStr"/>
-      <c r="AB96" t="inlineStr"/>
-      <c r="AC96" t="inlineStr"/>
-      <c r="AD96" t="inlineStr"/>
-      <c r="AE96" t="inlineStr"/>
-      <c r="AF96" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr"/>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>log_9</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>data('log').substring(540000,600000) == '' ? ' ' : data('log').substring(540000,600000)</t>
-        </is>
-      </c>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
-      <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr"/>
-      <c r="R97" t="inlineStr"/>
-      <c r="S97" t="inlineStr"/>
-      <c r="T97" t="inlineStr"/>
-      <c r="U97" t="inlineStr"/>
-      <c r="V97" t="inlineStr"/>
-      <c r="W97" t="inlineStr"/>
-      <c r="X97" t="inlineStr"/>
-      <c r="Y97" t="inlineStr"/>
-      <c r="Z97" t="inlineStr"/>
-      <c r="AA97" t="inlineStr"/>
-      <c r="AB97" t="inlineStr"/>
-      <c r="AC97" t="inlineStr"/>
-      <c r="AD97" t="inlineStr"/>
-      <c r="AE97" t="inlineStr"/>
-      <c r="AF97" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr"/>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>log_10</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>data('log').substring(600000,660000) == '' ? ' ' : data('log').substring(600000,660000)</t>
-        </is>
-      </c>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr"/>
-      <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
-      <c r="T98" t="inlineStr"/>
-      <c r="U98" t="inlineStr"/>
-      <c r="V98" t="inlineStr"/>
-      <c r="W98" t="inlineStr"/>
-      <c r="X98" t="inlineStr"/>
-      <c r="Y98" t="inlineStr"/>
-      <c r="Z98" t="inlineStr"/>
-      <c r="AA98" t="inlineStr"/>
-      <c r="AB98" t="inlineStr"/>
-      <c r="AC98" t="inlineStr"/>
-      <c r="AD98" t="inlineStr"/>
-      <c r="AE98" t="inlineStr"/>
-      <c r="AF98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr"/>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>log_11</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>data('log').substring(660000,720000) == '' ? ' ' : data('log').substring(660000,720000)</t>
-        </is>
-      </c>
-      <c r="J99" t="inlineStr"/>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr"/>
-      <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr"/>
-      <c r="P99" t="inlineStr"/>
-      <c r="Q99" t="inlineStr"/>
-      <c r="R99" t="inlineStr"/>
-      <c r="S99" t="inlineStr"/>
-      <c r="T99" t="inlineStr"/>
-      <c r="U99" t="inlineStr"/>
-      <c r="V99" t="inlineStr"/>
-      <c r="W99" t="inlineStr"/>
-      <c r="X99" t="inlineStr"/>
-      <c r="Y99" t="inlineStr"/>
-      <c r="Z99" t="inlineStr"/>
-      <c r="AA99" t="inlineStr"/>
-      <c r="AB99" t="inlineStr"/>
-      <c r="AC99" t="inlineStr"/>
-      <c r="AD99" t="inlineStr"/>
-      <c r="AE99" t="inlineStr"/>
-      <c r="AF99" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr"/>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>log_12</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr"/>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>data('log').substring(720000,780000) == '' ? ' ' : data('log').substring(720000,780000)</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr"/>
-      <c r="M100" t="inlineStr"/>
-      <c r="N100" t="inlineStr"/>
-      <c r="O100" t="inlineStr"/>
-      <c r="P100" t="inlineStr"/>
-      <c r="Q100" t="inlineStr"/>
-      <c r="R100" t="inlineStr"/>
-      <c r="S100" t="inlineStr"/>
-      <c r="T100" t="inlineStr"/>
-      <c r="U100" t="inlineStr"/>
-      <c r="V100" t="inlineStr"/>
-      <c r="W100" t="inlineStr"/>
-      <c r="X100" t="inlineStr"/>
-      <c r="Y100" t="inlineStr"/>
-      <c r="Z100" t="inlineStr"/>
-      <c r="AA100" t="inlineStr"/>
-      <c r="AB100" t="inlineStr"/>
-      <c r="AC100" t="inlineStr"/>
-      <c r="AD100" t="inlineStr"/>
-      <c r="AE100" t="inlineStr"/>
-      <c r="AF100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr"/>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>log_13</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>data('log').substring(780000,840000) == '' ? ' ' : data('log').substring(780000,840000)</t>
-        </is>
-      </c>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr"/>
-      <c r="P101" t="inlineStr"/>
-      <c r="Q101" t="inlineStr"/>
-      <c r="R101" t="inlineStr"/>
-      <c r="S101" t="inlineStr"/>
-      <c r="T101" t="inlineStr"/>
-      <c r="U101" t="inlineStr"/>
-      <c r="V101" t="inlineStr"/>
-      <c r="W101" t="inlineStr"/>
-      <c r="X101" t="inlineStr"/>
-      <c r="Y101" t="inlineStr"/>
-      <c r="Z101" t="inlineStr"/>
-      <c r="AA101" t="inlineStr"/>
-      <c r="AB101" t="inlineStr"/>
-      <c r="AC101" t="inlineStr"/>
-      <c r="AD101" t="inlineStr"/>
-      <c r="AE101" t="inlineStr"/>
-      <c r="AF101" t="inlineStr"/>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr"/>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>log_14</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr"/>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>data('log').substring(840000,900000) == '' ? ' ' : data('log').substring(840000,900000)</t>
-        </is>
-      </c>
-      <c r="J102" t="inlineStr"/>
-      <c r="K102" t="inlineStr"/>
-      <c r="L102" t="inlineStr"/>
-      <c r="M102" t="inlineStr"/>
-      <c r="N102" t="inlineStr"/>
-      <c r="O102" t="inlineStr"/>
-      <c r="P102" t="inlineStr"/>
-      <c r="Q102" t="inlineStr"/>
-      <c r="R102" t="inlineStr"/>
-      <c r="S102" t="inlineStr"/>
-      <c r="T102" t="inlineStr"/>
-      <c r="U102" t="inlineStr"/>
-      <c r="V102" t="inlineStr"/>
-      <c r="W102" t="inlineStr"/>
-      <c r="X102" t="inlineStr"/>
-      <c r="Y102" t="inlineStr"/>
-      <c r="Z102" t="inlineStr"/>
-      <c r="AA102" t="inlineStr"/>
-      <c r="AB102" t="inlineStr"/>
-      <c r="AC102" t="inlineStr"/>
-      <c r="AD102" t="inlineStr"/>
-      <c r="AE102" t="inlineStr"/>
-      <c r="AF102" t="inlineStr"/>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr"/>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>log_15</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr"/>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>data('log').substring(900000,960000) == '' ? ' ' : data('log').substring(900000,960000)</t>
-        </is>
-      </c>
-      <c r="J103" t="inlineStr"/>
-      <c r="K103" t="inlineStr"/>
-      <c r="L103" t="inlineStr"/>
-      <c r="M103" t="inlineStr"/>
-      <c r="N103" t="inlineStr"/>
-      <c r="O103" t="inlineStr"/>
-      <c r="P103" t="inlineStr"/>
-      <c r="Q103" t="inlineStr"/>
-      <c r="R103" t="inlineStr"/>
-      <c r="S103" t="inlineStr"/>
-      <c r="T103" t="inlineStr"/>
-      <c r="U103" t="inlineStr"/>
-      <c r="V103" t="inlineStr"/>
-      <c r="W103" t="inlineStr"/>
-      <c r="X103" t="inlineStr"/>
-      <c r="Y103" t="inlineStr"/>
-      <c r="Z103" t="inlineStr"/>
-      <c r="AA103" t="inlineStr"/>
-      <c r="AB103" t="inlineStr"/>
-      <c r="AC103" t="inlineStr"/>
-      <c r="AD103" t="inlineStr"/>
-      <c r="AE103" t="inlineStr"/>
-      <c r="AF103" t="inlineStr"/>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr"/>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>log_16</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr"/>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>data('log').substring(960000,1020000) == '' ? ' ' : data('log').substring(960000,1020000)</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr"/>
-      <c r="L104" t="inlineStr"/>
-      <c r="M104" t="inlineStr"/>
-      <c r="N104" t="inlineStr"/>
-      <c r="O104" t="inlineStr"/>
-      <c r="P104" t="inlineStr"/>
-      <c r="Q104" t="inlineStr"/>
-      <c r="R104" t="inlineStr"/>
-      <c r="S104" t="inlineStr"/>
-      <c r="T104" t="inlineStr"/>
-      <c r="U104" t="inlineStr"/>
-      <c r="V104" t="inlineStr"/>
-      <c r="W104" t="inlineStr"/>
-      <c r="X104" t="inlineStr"/>
-      <c r="Y104" t="inlineStr"/>
-      <c r="Z104" t="inlineStr"/>
-      <c r="AA104" t="inlineStr"/>
-      <c r="AB104" t="inlineStr"/>
-      <c r="AC104" t="inlineStr"/>
-      <c r="AD104" t="inlineStr"/>
-      <c r="AE104" t="inlineStr"/>
-      <c r="AF104" t="inlineStr"/>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr"/>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>log_17</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>data('log').substring(1020000,1080000) == '' ? ' ' : data('log').substring(1020000,1080000)</t>
-        </is>
-      </c>
-      <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr"/>
-      <c r="L105" t="inlineStr"/>
-      <c r="M105" t="inlineStr"/>
-      <c r="N105" t="inlineStr"/>
-      <c r="O105" t="inlineStr"/>
-      <c r="P105" t="inlineStr"/>
-      <c r="Q105" t="inlineStr"/>
-      <c r="R105" t="inlineStr"/>
-      <c r="S105" t="inlineStr"/>
-      <c r="T105" t="inlineStr"/>
-      <c r="U105" t="inlineStr"/>
-      <c r="V105" t="inlineStr"/>
-      <c r="W105" t="inlineStr"/>
-      <c r="X105" t="inlineStr"/>
-      <c r="Y105" t="inlineStr"/>
-      <c r="Z105" t="inlineStr"/>
-      <c r="AA105" t="inlineStr"/>
-      <c r="AB105" t="inlineStr"/>
-      <c r="AC105" t="inlineStr"/>
-      <c r="AD105" t="inlineStr"/>
-      <c r="AE105" t="inlineStr"/>
-      <c r="AF105" t="inlineStr"/>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>log_18</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>data('log').substring(1080000,1140000) == '' ? ' ' : data('log').substring(1080000,1140000)</t>
-        </is>
-      </c>
-      <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr"/>
-      <c r="L106" t="inlineStr"/>
-      <c r="M106" t="inlineStr"/>
-      <c r="N106" t="inlineStr"/>
-      <c r="O106" t="inlineStr"/>
-      <c r="P106" t="inlineStr"/>
-      <c r="Q106" t="inlineStr"/>
-      <c r="R106" t="inlineStr"/>
-      <c r="S106" t="inlineStr"/>
-      <c r="T106" t="inlineStr"/>
-      <c r="U106" t="inlineStr"/>
-      <c r="V106" t="inlineStr"/>
-      <c r="W106" t="inlineStr"/>
-      <c r="X106" t="inlineStr"/>
-      <c r="Y106" t="inlineStr"/>
-      <c r="Z106" t="inlineStr"/>
-      <c r="AA106" t="inlineStr"/>
-      <c r="AB106" t="inlineStr"/>
-      <c r="AC106" t="inlineStr"/>
-      <c r="AD106" t="inlineStr"/>
-      <c r="AE106" t="inlineStr"/>
-      <c r="AF106" t="inlineStr"/>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr"/>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr"/>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>assign</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>log_19</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr"/>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>data('log').substring(1140000,1200000) == '' ? ' ' : data('log').substring(1140000,1200000)</t>
-        </is>
-      </c>
-      <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr"/>
-      <c r="L107" t="inlineStr"/>
-      <c r="M107" t="inlineStr"/>
-      <c r="N107" t="inlineStr"/>
-      <c r="O107" t="inlineStr"/>
-      <c r="P107" t="inlineStr"/>
-      <c r="Q107" t="inlineStr"/>
-      <c r="R107" t="inlineStr"/>
-      <c r="S107" t="inlineStr"/>
-      <c r="T107" t="inlineStr"/>
-      <c r="U107" t="inlineStr"/>
-      <c r="V107" t="inlineStr"/>
-      <c r="W107" t="inlineStr"/>
-      <c r="X107" t="inlineStr"/>
-      <c r="Y107" t="inlineStr"/>
-      <c r="Z107" t="inlineStr"/>
-      <c r="AA107" t="inlineStr"/>
-      <c r="AB107" t="inlineStr"/>
-      <c r="AC107" t="inlineStr"/>
-      <c r="AD107" t="inlineStr"/>
-      <c r="AE107" t="inlineStr"/>
-      <c r="AF107" t="inlineStr"/>
-    </row>
   </sheetData>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" useFirstPageNumber="1" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -5199,20 +3817,20 @@
       <selection activeCell="B10" activeCellId="1" sqref="A32:XFD32 B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="30.85546875"/>
-    <col customWidth="1" max="2" min="2" style="2" width="20"/>
-    <col customWidth="1" max="1025" min="3" style="2" width="8.7109375"/>
+    <col customWidth="1" max="1" min="1" style="12" width="30.85546875"/>
+    <col customWidth="1" max="2" min="2" style="12" width="20"/>
+    <col customWidth="1" max="1025" min="3" style="12" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>setting_name</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>value</t>
         </is>
@@ -5224,46 +3842,46 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>table_id</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>person</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>form_id</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="8" t="inlineStr">
         <is>
           <t>person</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>form_version</t>
         </is>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="inlineStr">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>survey</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="8" t="inlineStr">
         <is>
           <t>New Person</t>
         </is>
@@ -5295,10 +3913,10 @@
       <selection activeCell="G72" activeCellId="1" sqref="A32:XFD32 G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="43.5703125"/>
-    <col customWidth="1" max="1025" min="2" style="2" width="8.7109375"/>
+    <col customWidth="1" max="1" min="1" style="12" width="43.42578125"/>
+    <col customWidth="1" max="1025" min="2" style="12" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5745,303 +4363,660 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="71" zoomScaleNormal="71">
-      <selection activeCell="C35" activeCellId="1" sqref="A32:XFD32 C35"/>
+      <selection activeCell="B38" sqref="B38:C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.7109375"/>
+    <col customWidth="1" max="1025" min="1" style="12" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>choice_list_name</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>data_value</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>display.title.text</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>site</t>
+    <row customHeight="1" ht="15.75" r="3" s="12">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>adeke_azuka</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
+          <t>Adeke Azuka</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="12">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ondo</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ondo</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>site</t>
+          <t>awe_abimbola</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>Awe Abimbola</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="12">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Edo</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Edo</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>site</t>
+          <t>benedict_azuogu</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>Benedict Azuogu</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="12">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ebonyi</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Ebonyi</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+          <t>chuks_abejegah</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>Chuks Abejegah</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="12">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dauda_saheed</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>Dauda Saheed</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="12">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>edith_abejegah</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="inlineStr">
+        <is>
+          <t>Edith Abejegah</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="12">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ewenyi_blessing</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
+        <is>
+          <t>Ewenyi Blessing</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="12">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ibemesi_deborah</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>Ibemesi Deborah</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="12">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ifenyinwa_akamike</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="inlineStr">
+        <is>
+          <t>Ifenyinwa Akamike</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ifenyinwa_okafor</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="inlineStr">
+        <is>
+          <t>Ifenyinwa Okafor</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="12">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>iloke_chijioke</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="inlineStr">
+        <is>
+          <t>Iloke Chijioke</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="12">
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>kingsley_okeke</t>
+        </is>
+      </c>
+      <c r="C14" s="11" t="inlineStr">
+        <is>
+          <t>Kingsley Okeke</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="12">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nancy_igboke</t>
+        </is>
+      </c>
+      <c r="C15" s="11" t="inlineStr">
+        <is>
+          <t>Nancy Igboke</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="12">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>oke_clement_osigbodi</t>
+        </is>
+      </c>
+      <c r="C16" s="11" t="inlineStr">
+        <is>
+          <t>Oke Clement Osigbodi</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="12">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>okocha_yusuf</t>
+        </is>
+      </c>
+      <c r="C17" s="11" t="inlineStr">
+        <is>
+          <t>Okocha Yusuf</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="12">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>osagbaekhoe_austin</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>Osagbaekhoe Austin</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="12">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>patricia_otuh</t>
+        </is>
+      </c>
+      <c r="C19" s="11" t="inlineStr">
+        <is>
+          <t>Patricia Otuh</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="20" s="12">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>roseline_adeleye</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="inlineStr">
+        <is>
+          <t>Roseline Adeleye</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="21" s="12">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>umeokonkwo_chukwuma</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
+        <is>
+          <t>Umeokonkwo Chukwuma</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="22" s="12">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>una_alfred</t>
+        </is>
+      </c>
+      <c r="C22" s="11" t="inlineStr">
+        <is>
+          <t>Una Alfred</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Other (enter name)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>interviewer_name</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Test (Not real data)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>consent</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>consent</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
           <t>gender</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>gender</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>household</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Household</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>community</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Community</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nearest hospital</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Nearest hospital</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>dumpsite</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Dumpsite</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>traps</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Traps</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>rice_or_other_farm</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Rice or other farm</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>GPS_ID</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>garri_rice_or_grain_drying_spot</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Garri, rice or grain drying spot</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>photo_consent</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>marital_status</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>married_single_wife</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Married (single wife)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>marital_status</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>married_multiple_wives</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Married (multiple wives)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>marital_status</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>unmarried</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Unmarried</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>p_lassa</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>photo_consent</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>p_lassa</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>p_lassa</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>dont_know</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Don't know</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>survivor</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Survivor</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>primary_contact</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Primary Contact</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>secondary_contact</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Secondary Contact</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">naive </t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Naïve </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>cohort</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>dont_know</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Don't Know</t>
         </is>
       </c>
     </row>

</xml_diff>